<commit_message>
Fixed typo, file should be fill
</commit_message>
<xml_diff>
--- a/www/input/bubbleplot.xlsx
+++ b/www/input/bubbleplot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bzhang1/github/quickr/www/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EC205D-31C9-CC43-A6B0-1107A553CE3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F26A56-1AC4-0B40-856A-447F1163F1AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24960" yWindow="10540" windowWidth="35200" windowHeight="19720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>Employment in 2012 (thousands)</t>
   </si>
   <si>
-    <t>file.by.legend.name</t>
-  </si>
-  <si>
     <t>Per cent with tertiary degree</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>fig.1.height</t>
+  </si>
+  <si>
+    <t>fill.by.legend.name</t>
   </si>
 </sst>
 </file>
@@ -1536,7 +1536,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1547,14 +1547,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="19">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1">
         <v>8</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
@@ -1564,14 +1564,14 @@
     </row>
     <row r="2" spans="1:9" ht="19">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="14"/>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="8"/>
@@ -1663,10 +1663,10 @@
     </row>
     <row r="9" spans="1:9" ht="19">
       <c r="A9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1676,10 +1676,10 @@
     </row>
     <row r="10" spans="1:9" ht="19">
       <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1689,10 +1689,10 @@
     </row>
     <row r="11" spans="1:9" ht="19">
       <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1702,10 +1702,10 @@
     </row>
     <row r="12" spans="1:9" ht="19">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1715,10 +1715,10 @@
     </row>
     <row r="13" spans="1:9" ht="19">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="14" spans="1:9" ht="19">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>

</xml_diff>